<commit_message>
linear combination tries, report results
</commit_message>
<xml_diff>
--- a/data/output/results/results_machine_learning.xlsx
+++ b/data/output/results/results_machine_learning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\VS Code\WebDataProject\data\output\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22AAF36-281F-439C-85F9-A8307C69FFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96969C5-A574-42E5-801F-A79A23A4DC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{30AB2D51-806F-4434-81F8-733D20158AF7}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="49">
   <si>
     <t>Kurzbeschreibung</t>
   </si>
@@ -146,6 +146,84 @@
   </si>
   <si>
     <t>RMan</t>
+  </si>
+  <si>
+    <t>Std String</t>
+  </si>
+  <si>
+    <t>0:30:46.027</t>
+  </si>
+  <si>
+    <t>Class 1 :
+3.85 +
+[[4] BookTitleComparatorPreprocessedJaccard] * -0.23 +
+[[15] BookAuthorComparatorJaccard] * -1.61 +
+[[3] BookTitleComparatorPreprocessedEqual] * 0.57 +
+[[9] BookTitleComparatorPreprocessedJaroWinkler] * -1.58 +
+[[2] BookTitleComparatorLevenshtein] * 1.2  +
+[[13] BookTitleComparatorPreprocessedMongeElkan] * -1.27 +
+[[11] BookTitleComparatorPreprocessedSmithWaterman] * -0.05 +
+[[23] BookAuthorComparatorMongeElkan] * -1.5 +
+[[22] BookAuthorComparatorPreprocessedMongeElkan] * 1.22</t>
+  </si>
+  <si>
+    <t>PYEucl</t>
+  </si>
+  <si>
+    <t>PYMan</t>
+  </si>
+  <si>
+    <t>PJacc</t>
+  </si>
+  <si>
+    <t>PJaro</t>
+  </si>
+  <si>
+    <t>PJW</t>
+  </si>
+  <si>
+    <t>PME</t>
+  </si>
+  <si>
+    <t>PLev</t>
+  </si>
+  <si>
+    <t>Class 1 :
+6.57 +
+[[4] BookTitleComparatorPreprocessedJaccard] * -0.78 +
+[[3] BookTitleComparatorPreprocessedEqual] * -0.78 +
+[[9] BookTitleComparatorPreprocessedJaroWinkler] * -9.96 +
+[[10] BookTitleComparatorSmithWaterman] * -0 +
+[[20] BookAuthorComparatorPreprocessedJaro] * 1.16 +
+[[17] BookAuthorComparatorJaccard] * -1.41 +
+[[12] BookTitleComparatorPreprocessedMongeElkan] * 0.46 +
+[[23] BookAuthorComparatorMongeElkan] * -2 +
+[[5] BookTitleComparatorPreprocessedLevenshtein] * 2    +
+[[6] BookTitleComparatorJaro] * 3.08</t>
+  </si>
+  <si>
+    <t>0:12:47.447</t>
+  </si>
+  <si>
+    <t>1:48:37.636</t>
+  </si>
+  <si>
+    <t>Class 1 :
+4.58 +
+[[4] BookTitleComparatorPreprocessedJaccard] * -4.77 +
+[[3] BookTitleComparatorPreprocessedEqual] * 0.89 +
+[[2] BookTitleComparatorLevenshtein] * -1.07 +
+[[9] BookTitleComparatorSmithWaterman] * -0.01 +
+[[7] BookTitleComparatorJaroWinkler] * -5.94 +
+[[12] BookAuthorComparatorJaccard] * -1 +
+[[11] BookAuthorComparatorPreprocessedJaccard] * -0.16 +
+[[5] BookTitleComparatorPreprocessedLevenshtein] * 7.84</t>
+  </si>
+  <si>
+    <t>m. TF-IDF</t>
+  </si>
+  <si>
+    <t>p-</t>
   </si>
 </sst>
 </file>
@@ -199,7 +277,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="87">
+  <dxfs count="88">
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -207,199 +285,202 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -475,108 +556,109 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{911E2576-8522-44C0-BCC3-5C312CB23CEF}" name="Tabelle48" displayName="Tabelle48" ref="A1:AA1048576" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
-  <autoFilter ref="A1:AA1048576" xr:uid="{EFB900FC-E7FD-4C54-92DB-310147D0E881}"/>
-  <tableColumns count="27">
-    <tableColumn id="1" xr3:uid="{9A449D20-EF5D-43DD-9923-060E7B0851F9}" name="Kurzbeschreibung" dataDxfId="55"/>
-    <tableColumn id="2" xr3:uid="{80260EC4-C5A1-4F31-9626-44D4C43454AF}" name="TEq" dataDxfId="54"/>
-    <tableColumn id="16" xr3:uid="{F9886828-7973-4E9E-8FDB-6DFFAFE757C3}" name="TJacc" dataDxfId="53"/>
-    <tableColumn id="15" xr3:uid="{4BC10426-7F50-4A9D-836D-8C85C364023D}" name="TLev" dataDxfId="52"/>
-    <tableColumn id="14" xr3:uid="{BE5FC9F9-D281-45A6-AFDC-A44BE288566A}" name="TIDF" dataDxfId="51"/>
-    <tableColumn id="13" xr3:uid="{6B8833B7-263F-4461-BDEF-724568F47153}" name="TJaro" dataDxfId="50"/>
-    <tableColumn id="12" xr3:uid="{00F1407E-3142-4ADE-B398-4FFC563E2B51}" name="TJW" dataDxfId="49"/>
-    <tableColumn id="17" xr3:uid="{BE9273B7-96A3-4B9A-8DF6-549C2CD046E0}" name="TSW" dataDxfId="48"/>
-    <tableColumn id="18" xr3:uid="{42847779-7F6B-4C35-9183-654FE5FF4478}" name="TME" dataDxfId="47"/>
-    <tableColumn id="19" xr3:uid="{BE08D352-42A7-4E47-9F3F-C2465EC13BB3}" name="AJacc" dataDxfId="46"/>
-    <tableColumn id="20" xr3:uid="{B2586606-3E44-4A05-8E7D-5FC73E5E60E5}" name="ALev" dataDxfId="45"/>
-    <tableColumn id="21" xr3:uid="{8B2F02EF-2B5D-49A0-8FCD-4F6F554BE93C}" name="AJaro" dataDxfId="44"/>
-    <tableColumn id="22" xr3:uid="{95BFE03B-9849-43CC-8D26-F56D7C4A4043}" name="AJW" dataDxfId="43"/>
-    <tableColumn id="23" xr3:uid="{D564553D-95AC-4575-AB14-6002BD3FF6D6}" name="AME" dataDxfId="42"/>
-    <tableColumn id="25" xr3:uid="{ACF80489-D79E-474D-B383-7D2DC8C2425A}" name="GJacc" dataDxfId="41"/>
-    <tableColumn id="24" xr3:uid="{DF0BE49D-E1C4-4C2A-8660-F7FC3D9B4F3C}" name="REucl" dataDxfId="40"/>
-    <tableColumn id="26" xr3:uid="{D276A89B-B378-4596-AB8C-37E8963EB177}" name="RMan" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{91C86056-8BF1-42AF-BAE2-F97AD4F4DBA8}" name="Blocking" dataDxfId="38"/>
-    <tableColumn id="9" xr3:uid="{1FCDED5D-F851-4551-82E1-E476E24C7304}" name="finalThreshold" dataDxfId="37"/>
-    <tableColumn id="11" xr3:uid="{53B71D9D-BB31-4120-9B96-8761B3C958A4}" name="modelType" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{C5EBCAF9-A0BB-4FCE-AACC-33F159AD1BEA}" name="TraiSet" dataDxfId="35"/>
-    <tableColumn id="27" xr3:uid="{C4FE34CD-62AD-4796-BAFE-ED66DF8C11DE}" name="RedRatio" dataDxfId="34"/>
-    <tableColumn id="10" xr3:uid="{96051D4E-E782-4364-BC2A-FB71F1E20F5B}" name="Laufzeit" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{44AE651D-CCA2-4A27-B902-1DC28CF69F03}" name="Precision" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{83F2D22D-7761-46F2-868F-BED983E2598E}" name="Recall" dataDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{615AC6A8-8F73-4F8F-8CC8-E76A3F74047B}" name="F1" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{0176AC2D-68CD-4562-A3E8-38873385EBAA}" name="Matching Rule" dataDxfId="29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{911E2576-8522-44C0-BCC3-5C312CB23CEF}" name="Tabelle48" displayName="Tabelle48" ref="A1:X1048576" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86">
+  <autoFilter ref="A1:X1048576" xr:uid="{EFB900FC-E7FD-4C54-92DB-310147D0E881}"/>
+  <tableColumns count="24">
+    <tableColumn id="1" xr3:uid="{9A449D20-EF5D-43DD-9923-060E7B0851F9}" name="Kurzbeschreibung" dataDxfId="85"/>
+    <tableColumn id="2" xr3:uid="{80260EC4-C5A1-4F31-9626-44D4C43454AF}" name="TEq" dataDxfId="84"/>
+    <tableColumn id="16" xr3:uid="{F9886828-7973-4E9E-8FDB-6DFFAFE757C3}" name="TJacc" dataDxfId="83"/>
+    <tableColumn id="15" xr3:uid="{4BC10426-7F50-4A9D-836D-8C85C364023D}" name="TLev" dataDxfId="82"/>
+    <tableColumn id="14" xr3:uid="{BE5FC9F9-D281-45A6-AFDC-A44BE288566A}" name="TIDF" dataDxfId="81"/>
+    <tableColumn id="13" xr3:uid="{6B8833B7-263F-4461-BDEF-724568F47153}" name="TJaro" dataDxfId="80"/>
+    <tableColumn id="12" xr3:uid="{00F1407E-3142-4ADE-B398-4FFC563E2B51}" name="TJW" dataDxfId="79"/>
+    <tableColumn id="17" xr3:uid="{BE9273B7-96A3-4B9A-8DF6-549C2CD046E0}" name="TSW" dataDxfId="78"/>
+    <tableColumn id="18" xr3:uid="{42847779-7F6B-4C35-9183-654FE5FF4478}" name="TME" dataDxfId="77"/>
+    <tableColumn id="19" xr3:uid="{BE08D352-42A7-4E47-9F3F-C2465EC13BB3}" name="AJacc" dataDxfId="76"/>
+    <tableColumn id="20" xr3:uid="{B2586606-3E44-4A05-8E7D-5FC73E5E60E5}" name="ALev" dataDxfId="75"/>
+    <tableColumn id="21" xr3:uid="{8B2F02EF-2B5D-49A0-8FCD-4F6F554BE93C}" name="AJaro" dataDxfId="74"/>
+    <tableColumn id="22" xr3:uid="{95BFE03B-9849-43CC-8D26-F56D7C4A4043}" name="AJW" dataDxfId="73"/>
+    <tableColumn id="23" xr3:uid="{D564553D-95AC-4575-AB14-6002BD3FF6D6}" name="AME" dataDxfId="72"/>
+    <tableColumn id="3" xr3:uid="{91C86056-8BF1-42AF-BAE2-F97AD4F4DBA8}" name="Blocking" dataDxfId="71"/>
+    <tableColumn id="9" xr3:uid="{1FCDED5D-F851-4551-82E1-E476E24C7304}" name="finalThreshold" dataDxfId="70"/>
+    <tableColumn id="11" xr3:uid="{53B71D9D-BB31-4120-9B96-8761B3C958A4}" name="modelType" dataDxfId="69"/>
+    <tableColumn id="4" xr3:uid="{C5EBCAF9-A0BB-4FCE-AACC-33F159AD1BEA}" name="TraiSet" dataDxfId="68"/>
+    <tableColumn id="27" xr3:uid="{C4FE34CD-62AD-4796-BAFE-ED66DF8C11DE}" name="RedRatio" dataDxfId="67"/>
+    <tableColumn id="10" xr3:uid="{96051D4E-E782-4364-BC2A-FB71F1E20F5B}" name="Laufzeit" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{44AE651D-CCA2-4A27-B902-1DC28CF69F03}" name="Precision" dataDxfId="65"/>
+    <tableColumn id="7" xr3:uid="{83F2D22D-7761-46F2-868F-BED983E2598E}" name="Recall" dataDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{615AC6A8-8F73-4F8F-8CC8-E76A3F74047B}" name="F1" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{0176AC2D-68CD-4562-A3E8-38873385EBAA}" name="Matching Rule" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{EFB900FC-E7FD-4C54-92DB-310147D0E881}" name="Tabelle4" displayName="Tabelle4" ref="A1:AA1048576" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{EFB900FC-E7FD-4C54-92DB-310147D0E881}" name="Tabelle4" displayName="Tabelle4" ref="A1:AA1048576" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <autoFilter ref="A1:AA1048576" xr:uid="{EFB900FC-E7FD-4C54-92DB-310147D0E881}"/>
   <tableColumns count="27">
-    <tableColumn id="1" xr3:uid="{984DB0C4-F125-4AD8-BA6B-DFA4355BA94F}" name="Kurzbeschreibung" dataDxfId="86"/>
-    <tableColumn id="2" xr3:uid="{20787FF6-86EA-4FA5-81B4-71210AE17080}" name="TEq" dataDxfId="85"/>
-    <tableColumn id="16" xr3:uid="{E60F5B8B-6C74-4FCF-91D7-2CD571FA3D47}" name="TJacc" dataDxfId="84"/>
-    <tableColumn id="15" xr3:uid="{2DF062E9-71C8-4C57-AFA6-9A7F2A05B01E}" name="TLev" dataDxfId="83"/>
-    <tableColumn id="14" xr3:uid="{AB0A4BDB-750C-4DEE-A18F-C5C74FBF7CBE}" name="TIDF" dataDxfId="82"/>
-    <tableColumn id="13" xr3:uid="{B0A6ECB1-E40A-4FA4-984B-4D15F6665EA2}" name="TJaro" dataDxfId="81"/>
-    <tableColumn id="12" xr3:uid="{86BB775B-D7B9-4DEC-812F-1801AEA898D4}" name="TJW" dataDxfId="80"/>
-    <tableColumn id="17" xr3:uid="{B85AE136-61A1-4409-A05A-FB83E429A805}" name="TSW" dataDxfId="79"/>
-    <tableColumn id="18" xr3:uid="{9A2CBF10-F79E-4C7F-9D01-6CDCD6ED809F}" name="TME" dataDxfId="78"/>
-    <tableColumn id="19" xr3:uid="{42995688-2C69-4700-8481-D7403B927FE4}" name="AJacc" dataDxfId="77"/>
-    <tableColumn id="20" xr3:uid="{3EF6EE55-7438-4D62-9022-C6F8B2A4C5C6}" name="ALev" dataDxfId="76"/>
-    <tableColumn id="21" xr3:uid="{B8A81252-8E3F-41B0-8A0E-1289BD2273D6}" name="AJaro" dataDxfId="75"/>
-    <tableColumn id="22" xr3:uid="{95E62EEB-2FCF-4BFB-BD86-93B5F169CC4E}" name="AJW" dataDxfId="74"/>
-    <tableColumn id="23" xr3:uid="{96692E27-467D-4652-8DC6-4EDF66996934}" name="AME" dataDxfId="73"/>
-    <tableColumn id="25" xr3:uid="{57FB89EA-965A-42C7-B655-EFE282941E57}" name="GJacc" dataDxfId="72"/>
-    <tableColumn id="24" xr3:uid="{B7034EE0-CD71-4AE7-9C5B-D5C966D64C97}" name="REucl" dataDxfId="71"/>
-    <tableColumn id="26" xr3:uid="{DBBB1DA6-1605-4015-AE27-279B32171388}" name="RMan" dataDxfId="70"/>
-    <tableColumn id="3" xr3:uid="{40957401-40E3-486C-A03B-02EB0C5FF500}" name="Blocking" dataDxfId="69"/>
-    <tableColumn id="9" xr3:uid="{A4064A98-9BE5-4CE9-A3E4-76CEF3A41A7E}" name="finalThreshold" dataDxfId="68"/>
-    <tableColumn id="11" xr3:uid="{BD5C3BA8-9874-4B29-828E-0BC28A95C02E}" name="modelType" dataDxfId="67"/>
-    <tableColumn id="4" xr3:uid="{0A7F8DF5-8A5C-418E-81F9-46CFE51EE589}" name="TraiSet" dataDxfId="66"/>
-    <tableColumn id="27" xr3:uid="{B6AC362D-211C-4EC0-9098-172BA4569854}" name="RedRatio" dataDxfId="60"/>
-    <tableColumn id="10" xr3:uid="{0463B6E8-B83D-4F4A-AF5F-B8655D3414A5}" name="Laufzeit" dataDxfId="65"/>
-    <tableColumn id="6" xr3:uid="{06F7F68F-F8C8-4054-8DAF-C1BD36BFA73F}" name="Precision" dataDxfId="64"/>
-    <tableColumn id="7" xr3:uid="{61987D4F-9AE0-4844-8200-30F7C1758B0C}" name="Recall" dataDxfId="63"/>
-    <tableColumn id="8" xr3:uid="{FD6EF029-0858-408D-8496-F6AB7F497486}" name="F1" dataDxfId="58"/>
-    <tableColumn id="5" xr3:uid="{26BAC032-B233-4050-A08C-C74A953B3C7B}" name="Matching Rule" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{984DB0C4-F125-4AD8-BA6B-DFA4355BA94F}" name="Kurzbeschreibung" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{20787FF6-86EA-4FA5-81B4-71210AE17080}" name="TEq" dataDxfId="58"/>
+    <tableColumn id="16" xr3:uid="{E60F5B8B-6C74-4FCF-91D7-2CD571FA3D47}" name="TJacc" dataDxfId="57"/>
+    <tableColumn id="15" xr3:uid="{2DF062E9-71C8-4C57-AFA6-9A7F2A05B01E}" name="TLev" dataDxfId="56"/>
+    <tableColumn id="14" xr3:uid="{AB0A4BDB-750C-4DEE-A18F-C5C74FBF7CBE}" name="TIDF" dataDxfId="55"/>
+    <tableColumn id="13" xr3:uid="{B0A6ECB1-E40A-4FA4-984B-4D15F6665EA2}" name="TJaro" dataDxfId="54"/>
+    <tableColumn id="12" xr3:uid="{86BB775B-D7B9-4DEC-812F-1801AEA898D4}" name="TJW" dataDxfId="53"/>
+    <tableColumn id="17" xr3:uid="{B85AE136-61A1-4409-A05A-FB83E429A805}" name="TSW" dataDxfId="52"/>
+    <tableColumn id="18" xr3:uid="{9A2CBF10-F79E-4C7F-9D01-6CDCD6ED809F}" name="TME" dataDxfId="51"/>
+    <tableColumn id="19" xr3:uid="{42995688-2C69-4700-8481-D7403B927FE4}" name="AJacc" dataDxfId="50"/>
+    <tableColumn id="20" xr3:uid="{3EF6EE55-7438-4D62-9022-C6F8B2A4C5C6}" name="ALev" dataDxfId="49"/>
+    <tableColumn id="21" xr3:uid="{B8A81252-8E3F-41B0-8A0E-1289BD2273D6}" name="AJaro" dataDxfId="48"/>
+    <tableColumn id="22" xr3:uid="{95E62EEB-2FCF-4BFB-BD86-93B5F169CC4E}" name="AJW" dataDxfId="47"/>
+    <tableColumn id="23" xr3:uid="{96692E27-467D-4652-8DC6-4EDF66996934}" name="AME" dataDxfId="46"/>
+    <tableColumn id="25" xr3:uid="{57FB89EA-965A-42C7-B655-EFE282941E57}" name="GJacc" dataDxfId="45"/>
+    <tableColumn id="24" xr3:uid="{B7034EE0-CD71-4AE7-9C5B-D5C966D64C97}" name="REucl" dataDxfId="44"/>
+    <tableColumn id="26" xr3:uid="{DBBB1DA6-1605-4015-AE27-279B32171388}" name="RMan" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{40957401-40E3-486C-A03B-02EB0C5FF500}" name="Blocking" dataDxfId="42"/>
+    <tableColumn id="9" xr3:uid="{A4064A98-9BE5-4CE9-A3E4-76CEF3A41A7E}" name="finalThreshold" dataDxfId="41"/>
+    <tableColumn id="11" xr3:uid="{BD5C3BA8-9874-4B29-828E-0BC28A95C02E}" name="modelType" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{0A7F8DF5-8A5C-418E-81F9-46CFE51EE589}" name="TraiSet" dataDxfId="39"/>
+    <tableColumn id="27" xr3:uid="{B6AC362D-211C-4EC0-9098-172BA4569854}" name="RedRatio" dataDxfId="38"/>
+    <tableColumn id="10" xr3:uid="{0463B6E8-B83D-4F4A-AF5F-B8655D3414A5}" name="Laufzeit" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{06F7F68F-F8C8-4054-8DAF-C1BD36BFA73F}" name="Precision" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{61987D4F-9AE0-4844-8200-30F7C1758B0C}" name="Recall" dataDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{FD6EF029-0858-408D-8496-F6AB7F497486}" name="F1" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{26BAC032-B233-4050-A08C-C74A953B3C7B}" name="Matching Rule" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4F6E5481-84FC-4FEF-B9E4-4AB9203E0862}" name="Tabelle49" displayName="Tabelle49" ref="A1:AA1048576" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
-  <autoFilter ref="A1:AA1048576" xr:uid="{EFB900FC-E7FD-4C54-92DB-310147D0E881}"/>
-  <tableColumns count="27">
-    <tableColumn id="1" xr3:uid="{DFE2D2E8-3291-4CFF-80D8-984D534D53AB}" name="Kurzbeschreibung" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{3DF416F4-B031-47B0-B16B-2B4B18461AAE}" name="TEq" dataDxfId="25"/>
-    <tableColumn id="16" xr3:uid="{32E2DB63-397E-4FCA-850D-6B86C3C04E32}" name="TJacc" dataDxfId="24"/>
-    <tableColumn id="15" xr3:uid="{2EE596CF-0AED-43AD-A102-D1B008E4996D}" name="TLev" dataDxfId="23"/>
-    <tableColumn id="14" xr3:uid="{50595DA5-FB7F-4B02-8A7A-80068DFA4297}" name="TIDF" dataDxfId="22"/>
-    <tableColumn id="13" xr3:uid="{1E0D9BC8-A041-494B-9EFD-EDFDCF98C1FA}" name="TJaro" dataDxfId="21"/>
-    <tableColumn id="12" xr3:uid="{04DCEFC3-A31F-4430-9CDD-B7BE34F21A76}" name="TJW" dataDxfId="20"/>
-    <tableColumn id="17" xr3:uid="{CAA9C079-C858-4A66-B806-AF6D9C19731D}" name="TSW" dataDxfId="19"/>
-    <tableColumn id="18" xr3:uid="{C719E628-2B4C-4F33-873C-BDB8C386081B}" name="TME" dataDxfId="18"/>
-    <tableColumn id="19" xr3:uid="{9A1F1268-F66B-4C5C-8D61-DF098DDD8ECC}" name="AJacc" dataDxfId="17"/>
-    <tableColumn id="20" xr3:uid="{F6E2D9EA-388E-41EA-90B0-8C942BC352DA}" name="ALev" dataDxfId="16"/>
-    <tableColumn id="21" xr3:uid="{C36AC9B9-51ED-49DE-92A9-AA6960429144}" name="AJaro" dataDxfId="15"/>
-    <tableColumn id="22" xr3:uid="{EF62FBAA-99B3-45E6-A7E7-D7CE372E5EC3}" name="AJW" dataDxfId="14"/>
-    <tableColumn id="23" xr3:uid="{519EA73C-33D3-4392-9C26-489C54861CF3}" name="AME" dataDxfId="13"/>
-    <tableColumn id="25" xr3:uid="{AB0D6F20-2570-4E55-B91D-C486B8CB7B96}" name="GJacc" dataDxfId="12"/>
-    <tableColumn id="24" xr3:uid="{2A29D0B8-C971-4093-8045-1D77CA82F0EF}" name="REucl" dataDxfId="11"/>
-    <tableColumn id="26" xr3:uid="{46A98AE6-FF37-46EF-A207-714365B3C94D}" name="RMan" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{051850A1-BE40-4060-B556-59C2C8B4BE9A}" name="Blocking" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{62FAA148-403D-431B-8011-6230EEB9CA66}" name="finalThreshold" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{A3B60CD6-06D4-4D3C-853E-679F15AB31DB}" name="modelType" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{53F469BB-A7A8-442E-9FF1-50D47CA475EF}" name="TraiSet" dataDxfId="6"/>
-    <tableColumn id="27" xr3:uid="{951ABBF0-7713-43E7-9EAA-CA1F92EE5F6A}" name="RedRatio" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{02EB987A-8EA0-4008-BBE2-3C48B5982835}" name="Laufzeit" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{14E74792-F467-4B37-B462-CE73C2BFFAE8}" name="Precision" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{E413E5C9-F387-418B-B704-96D934E358C0}" name="Recall" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{6E418D7A-1E79-4B12-9595-C5447DF6D8F9}" name="F1" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{8898F28D-E3FF-4251-852B-98C9322C3E9F}" name="Matching Rule" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4F6E5481-84FC-4FEF-B9E4-4AB9203E0862}" name="Tabelle49" displayName="Tabelle49" ref="A1:AE1048576" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+  <autoFilter ref="A1:AE1048576" xr:uid="{EFB900FC-E7FD-4C54-92DB-310147D0E881}"/>
+  <tableColumns count="31">
+    <tableColumn id="1" xr3:uid="{DFE2D2E8-3291-4CFF-80D8-984D534D53AB}" name="Kurzbeschreibung" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{3DF416F4-B031-47B0-B16B-2B4B18461AAE}" name="TEq" dataDxfId="29"/>
+    <tableColumn id="16" xr3:uid="{32E2DB63-397E-4FCA-850D-6B86C3C04E32}" name="TJacc" dataDxfId="28"/>
+    <tableColumn id="15" xr3:uid="{2EE596CF-0AED-43AD-A102-D1B008E4996D}" name="TLev" dataDxfId="27"/>
+    <tableColumn id="14" xr3:uid="{50595DA5-FB7F-4B02-8A7A-80068DFA4297}" name="TIDF" dataDxfId="26"/>
+    <tableColumn id="13" xr3:uid="{1E0D9BC8-A041-494B-9EFD-EDFDCF98C1FA}" name="TJaro" dataDxfId="25"/>
+    <tableColumn id="12" xr3:uid="{04DCEFC3-A31F-4430-9CDD-B7BE34F21A76}" name="TJW" dataDxfId="24"/>
+    <tableColumn id="17" xr3:uid="{CAA9C079-C858-4A66-B806-AF6D9C19731D}" name="TSW" dataDxfId="23"/>
+    <tableColumn id="18" xr3:uid="{C719E628-2B4C-4F33-873C-BDB8C386081B}" name="TME" dataDxfId="22"/>
+    <tableColumn id="35" xr3:uid="{57C54906-553D-4B6F-B7E7-A8E031F5AA83}" name="PJacc" dataDxfId="4"/>
+    <tableColumn id="36" xr3:uid="{3534D14F-F788-4521-AC30-73DF35EDE914}" name="PLev" dataDxfId="3"/>
+    <tableColumn id="38" xr3:uid="{65500E02-1F80-443C-8746-3B36C1AE9806}" name="PJaro" dataDxfId="2"/>
+    <tableColumn id="39" xr3:uid="{D81EFF64-5236-4256-AFA4-265BC9704013}" name="PJW" dataDxfId="1"/>
+    <tableColumn id="41" xr3:uid="{CD201A4A-0F39-4401-B87D-6629CD810346}" name="PME" dataDxfId="0"/>
+    <tableColumn id="19" xr3:uid="{9A1F1268-F66B-4C5C-8D61-DF098DDD8ECC}" name="AJacc" dataDxfId="21"/>
+    <tableColumn id="20" xr3:uid="{F6E2D9EA-388E-41EA-90B0-8C942BC352DA}" name="ALev" dataDxfId="20"/>
+    <tableColumn id="21" xr3:uid="{C36AC9B9-51ED-49DE-92A9-AA6960429144}" name="AJaro" dataDxfId="19"/>
+    <tableColumn id="22" xr3:uid="{EF62FBAA-99B3-45E6-A7E7-D7CE372E5EC3}" name="AJW" dataDxfId="18"/>
+    <tableColumn id="23" xr3:uid="{519EA73C-33D3-4392-9C26-489C54861CF3}" name="AME" dataDxfId="17"/>
+    <tableColumn id="24" xr3:uid="{2A29D0B8-C971-4093-8045-1D77CA82F0EF}" name="PYEucl" dataDxfId="16"/>
+    <tableColumn id="26" xr3:uid="{46A98AE6-FF37-46EF-A207-714365B3C94D}" name="PYMan" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{051850A1-BE40-4060-B556-59C2C8B4BE9A}" name="Blocking" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{62FAA148-403D-431B-8011-6230EEB9CA66}" name="finalThreshold" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{A3B60CD6-06D4-4D3C-853E-679F15AB31DB}" name="modelType" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{53F469BB-A7A8-442E-9FF1-50D47CA475EF}" name="TraiSet" dataDxfId="11"/>
+    <tableColumn id="27" xr3:uid="{951ABBF0-7713-43E7-9EAA-CA1F92EE5F6A}" name="RedRatio" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{02EB987A-8EA0-4008-BBE2-3C48B5982835}" name="Laufzeit" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{14E74792-F467-4B37-B462-CE73C2BFFAE8}" name="Precision" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{E413E5C9-F387-418B-B704-96D934E358C0}" name="Recall" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{6E418D7A-1E79-4B12-9595-C5447DF6D8F9}" name="F1" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{8898F28D-E3FF-4251-852B-98C9322C3E9F}" name="Matching Rule" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -879,10 +961,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2438B34D-286C-4535-84FF-1F263F006FB3}">
-  <dimension ref="A1:AA2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" style="1" customWidth="1"/>
+    <col min="21" max="23" width="11.42578125" style="1"/>
+    <col min="24" max="24" width="55.42578125" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="210" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" s="1">
+        <v>1</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0.99991521007530204</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="V2" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="W2" s="1">
+        <v>0.77780000000000005</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D980BE-ACF9-443A-81B5-F4AB23596DA5}">
+  <dimension ref="A1:AA3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,155 +1268,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="AA2" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D980BE-ACF9-443A-81B5-F4AB23596DA5}">
-  <dimension ref="A1:AA2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.42578125" style="1" customWidth="1"/>
-    <col min="24" max="26" width="11.42578125" style="1"/>
-    <col min="27" max="27" width="55.42578125" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="11.42578125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="2" spans="1:27" ht="150" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>11</v>
@@ -1225,6 +1346,89 @@
       </c>
       <c r="AA2" s="2" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="150" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="U3" s="1">
+        <v>1</v>
+      </c>
+      <c r="V3" s="2">
+        <v>0.99944443380141301</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X3" s="1">
+        <v>0.92310000000000003</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>0.8276</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1238,7 +1442,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{709E18BA-5481-45E6-BF80-7E9C396A1CBD}">
-  <dimension ref="A1:AA2"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1255,26 +1459,30 @@
     <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.42578125" style="1" customWidth="1"/>
-    <col min="24" max="26" width="11.42578125" style="1"/>
-    <col min="27" max="27" width="55.42578125" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="11.42578125" style="1"/>
+    <col min="10" max="10" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.42578125" style="1" customWidth="1"/>
+    <col min="28" max="30" width="11.42578125" style="1"/>
+    <col min="31" max="31" width="55.42578125" style="1" customWidth="1"/>
+    <col min="32" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1303,81 +1511,166 @@
         <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="AA2" s="2"/>
+    <row r="2" spans="1:31" ht="195" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>0.99990288541264105</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>0.95650000000000002</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>0.73329999999999995</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>0.83020000000000005</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
checked with threshold 0.7
</commit_message>
<xml_diff>
--- a/data/output/results/results_machine_learning.xlsx
+++ b/data/output/results/results_machine_learning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\VS Code\WebDataProject\data\output\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96969C5-A574-42E5-801F-A79A23A4DC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11787FBB-4A18-4054-B2B7-E01C898826BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{30AB2D51-806F-4434-81F8-733D20158AF7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{30AB2D51-806F-4434-81F8-733D20158AF7}"/>
   </bookViews>
   <sheets>
     <sheet name="AmazCov" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="52">
   <si>
     <t>Kurzbeschreibung</t>
   </si>
@@ -224,6 +224,15 @@
   </si>
   <si>
     <t>p-</t>
+  </si>
+  <si>
+    <t>threshold 0,7</t>
+  </si>
+  <si>
+    <t>0:04:26.095</t>
+  </si>
+  <si>
+    <t>0:12:20.514</t>
   </si>
 </sst>
 </file>
@@ -285,9 +294,51 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -300,49 +351,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -637,28 +646,28 @@
     <tableColumn id="12" xr3:uid="{04DCEFC3-A31F-4430-9CDD-B7BE34F21A76}" name="TJW" dataDxfId="24"/>
     <tableColumn id="17" xr3:uid="{CAA9C079-C858-4A66-B806-AF6D9C19731D}" name="TSW" dataDxfId="23"/>
     <tableColumn id="18" xr3:uid="{C719E628-2B4C-4F33-873C-BDB8C386081B}" name="TME" dataDxfId="22"/>
-    <tableColumn id="35" xr3:uid="{57C54906-553D-4B6F-B7E7-A8E031F5AA83}" name="PJacc" dataDxfId="4"/>
-    <tableColumn id="36" xr3:uid="{3534D14F-F788-4521-AC30-73DF35EDE914}" name="PLev" dataDxfId="3"/>
-    <tableColumn id="38" xr3:uid="{65500E02-1F80-443C-8746-3B36C1AE9806}" name="PJaro" dataDxfId="2"/>
-    <tableColumn id="39" xr3:uid="{D81EFF64-5236-4256-AFA4-265BC9704013}" name="PJW" dataDxfId="1"/>
-    <tableColumn id="41" xr3:uid="{CD201A4A-0F39-4401-B87D-6629CD810346}" name="PME" dataDxfId="0"/>
-    <tableColumn id="19" xr3:uid="{9A1F1268-F66B-4C5C-8D61-DF098DDD8ECC}" name="AJacc" dataDxfId="21"/>
-    <tableColumn id="20" xr3:uid="{F6E2D9EA-388E-41EA-90B0-8C942BC352DA}" name="ALev" dataDxfId="20"/>
-    <tableColumn id="21" xr3:uid="{C36AC9B9-51ED-49DE-92A9-AA6960429144}" name="AJaro" dataDxfId="19"/>
-    <tableColumn id="22" xr3:uid="{EF62FBAA-99B3-45E6-A7E7-D7CE372E5EC3}" name="AJW" dataDxfId="18"/>
-    <tableColumn id="23" xr3:uid="{519EA73C-33D3-4392-9C26-489C54861CF3}" name="AME" dataDxfId="17"/>
-    <tableColumn id="24" xr3:uid="{2A29D0B8-C971-4093-8045-1D77CA82F0EF}" name="PYEucl" dataDxfId="16"/>
-    <tableColumn id="26" xr3:uid="{46A98AE6-FF37-46EF-A207-714365B3C94D}" name="PYMan" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{051850A1-BE40-4060-B556-59C2C8B4BE9A}" name="Blocking" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{62FAA148-403D-431B-8011-6230EEB9CA66}" name="finalThreshold" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{A3B60CD6-06D4-4D3C-853E-679F15AB31DB}" name="modelType" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{53F469BB-A7A8-442E-9FF1-50D47CA475EF}" name="TraiSet" dataDxfId="11"/>
-    <tableColumn id="27" xr3:uid="{951ABBF0-7713-43E7-9EAA-CA1F92EE5F6A}" name="RedRatio" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{02EB987A-8EA0-4008-BBE2-3C48B5982835}" name="Laufzeit" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{14E74792-F467-4B37-B462-CE73C2BFFAE8}" name="Precision" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{E413E5C9-F387-418B-B704-96D934E358C0}" name="Recall" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{6E418D7A-1E79-4B12-9595-C5447DF6D8F9}" name="F1" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{8898F28D-E3FF-4251-852B-98C9322C3E9F}" name="Matching Rule" dataDxfId="5"/>
+    <tableColumn id="35" xr3:uid="{57C54906-553D-4B6F-B7E7-A8E031F5AA83}" name="PJacc" dataDxfId="21"/>
+    <tableColumn id="36" xr3:uid="{3534D14F-F788-4521-AC30-73DF35EDE914}" name="PLev" dataDxfId="20"/>
+    <tableColumn id="38" xr3:uid="{65500E02-1F80-443C-8746-3B36C1AE9806}" name="PJaro" dataDxfId="19"/>
+    <tableColumn id="39" xr3:uid="{D81EFF64-5236-4256-AFA4-265BC9704013}" name="PJW" dataDxfId="18"/>
+    <tableColumn id="41" xr3:uid="{CD201A4A-0F39-4401-B87D-6629CD810346}" name="PME" dataDxfId="17"/>
+    <tableColumn id="19" xr3:uid="{9A1F1268-F66B-4C5C-8D61-DF098DDD8ECC}" name="AJacc" dataDxfId="16"/>
+    <tableColumn id="20" xr3:uid="{F6E2D9EA-388E-41EA-90B0-8C942BC352DA}" name="ALev" dataDxfId="15"/>
+    <tableColumn id="21" xr3:uid="{C36AC9B9-51ED-49DE-92A9-AA6960429144}" name="AJaro" dataDxfId="14"/>
+    <tableColumn id="22" xr3:uid="{EF62FBAA-99B3-45E6-A7E7-D7CE372E5EC3}" name="AJW" dataDxfId="13"/>
+    <tableColumn id="23" xr3:uid="{519EA73C-33D3-4392-9C26-489C54861CF3}" name="AME" dataDxfId="12"/>
+    <tableColumn id="24" xr3:uid="{2A29D0B8-C971-4093-8045-1D77CA82F0EF}" name="PYEucl" dataDxfId="11"/>
+    <tableColumn id="26" xr3:uid="{46A98AE6-FF37-46EF-A207-714365B3C94D}" name="PYMan" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{051850A1-BE40-4060-B556-59C2C8B4BE9A}" name="Blocking" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{62FAA148-403D-431B-8011-6230EEB9CA66}" name="finalThreshold" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{A3B60CD6-06D4-4D3C-853E-679F15AB31DB}" name="modelType" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{53F469BB-A7A8-442E-9FF1-50D47CA475EF}" name="TraiSet" dataDxfId="6"/>
+    <tableColumn id="27" xr3:uid="{951ABBF0-7713-43E7-9EAA-CA1F92EE5F6A}" name="RedRatio" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{02EB987A-8EA0-4008-BBE2-3C48B5982835}" name="Laufzeit" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{14E74792-F467-4B37-B462-CE73C2BFFAE8}" name="Precision" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{E413E5C9-F387-418B-B704-96D934E358C0}" name="Recall" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{6E418D7A-1E79-4B12-9595-C5447DF6D8F9}" name="F1" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{8898F28D-E3FF-4251-852B-98C9322C3E9F}" name="Matching Rule" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1149,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D980BE-ACF9-443A-81B5-F4AB23596DA5}">
-  <dimension ref="A1:AA3"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,6 +1440,89 @@
         <v>46</v>
       </c>
     </row>
+    <row r="4" spans="1:27" ht="150" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="U4" s="1">
+        <v>1</v>
+      </c>
+      <c r="V4" s="2">
+        <v>0.99944443380141301</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="X4" s="1">
+        <v>0.90480000000000005</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>0.59379999999999999</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1442,10 +1534,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{709E18BA-5481-45E6-BF80-7E9C396A1CBD}">
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="AE3" sqref="AE3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1669,6 +1761,101 @@
         <v>43</v>
       </c>
     </row>
+    <row r="3" spans="1:31" ht="195" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W3" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>0.99990288541264105</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>0.95450000000000002</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>0.80769999999999997</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>